<commit_message>
dashboard segunda update modificado de sus datos en server y cambio de zoom
</commit_message>
<xml_diff>
--- a/server/resources/data_dashboard_OLD.xlsx
+++ b/server/resources/data_dashboard_OLD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinh/Documents/Khora/Getafe/GetafeEPIUReact/server/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Miguel/Desktop/khora/proyecto_visor_Privado_EMSV/Visor_Privado_EMSV/server/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FEF6CD5-BF5E-9242-B4C7-BE1DBEAF90F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF2E884-C472-224D-B424-2849428F8B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="500" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{FF8EA80C-DBF0-45CC-B8AC-E813896C236E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16740" activeTab="5" xr2:uid="{FF8EA80C-DBF0-45CC-B8AC-E813896C236E}"/>
   </bookViews>
   <sheets>
     <sheet name="Contador" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="grafico secundario abajo dcha" sheetId="12" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Contador!$A$1:$C$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Contador!$A$1:$B$4</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="73">
   <si>
     <t>Usuarios de la OHS</t>
   </si>
@@ -91,18 +91,6 @@
     <t>% personas</t>
   </si>
   <si>
-    <t>Optimización de factura</t>
-  </si>
-  <si>
-    <t>Ayudas a rehabilitación</t>
-  </si>
-  <si>
-    <t>Información general</t>
-  </si>
-  <si>
-    <t>Bono Social</t>
-  </si>
-  <si>
     <t>Origen de los usuarios</t>
   </si>
   <si>
@@ -224,13 +212,64 @@
   </si>
   <si>
     <t>jul-23</t>
+  </si>
+  <si>
+    <t>ago-23</t>
+  </si>
+  <si>
+    <t>sep-23</t>
+  </si>
+  <si>
+    <t>oct-23</t>
+  </si>
+  <si>
+    <t>nov-23</t>
+  </si>
+  <si>
+    <t>Rehabilitación (IEE, ITEs,…)</t>
+  </si>
+  <si>
+    <t>Suministros (Agua, luz, gas)</t>
+  </si>
+  <si>
+    <t>Compra vivienda nueva</t>
+  </si>
+  <si>
+    <t>Alquiler vivienda nueva</t>
+  </si>
+  <si>
+    <t>Programas de alquiler</t>
+  </si>
+  <si>
+    <t>Plazas de garaje</t>
+  </si>
+  <si>
+    <t>Comunidades energéticas (OTC)</t>
+  </si>
+  <si>
+    <t>Autoconsumo</t>
+  </si>
+  <si>
+    <t>Convocatoria ascensores</t>
+  </si>
+  <si>
+    <t>Convocatorias eficiencia energética</t>
+  </si>
+  <si>
+    <t>Convocatorias rehabilitación</t>
+  </si>
+  <si>
+    <t>Convocatoria ayuda en suministros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Convocatoria de Alquiler </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,16 +309,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -296,57 +360,80 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -362,9 +449,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -402,7 +489,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -508,7 +595,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -650,7 +737,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -661,87 +748,49 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView showGridLines="0" zoomScale="157" zoomScaleNormal="99" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.5" style="2"/>
-    <col min="3" max="3" width="11.5" style="9"/>
-    <col min="4" max="16384" width="11.5" style="2"/>
+    <col min="1" max="1" width="17.83203125" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="11.5" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4">
-        <v>1349</v>
-      </c>
-      <c r="C1" s="8"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" s="14">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
-        <v>1675</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="15">
+        <v>1937</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
-        <v>2402</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B3" s="15">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
-        <v>307</v>
-      </c>
-      <c r="C4" s="7"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="7"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="7"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="7"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="7"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="7"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="7"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
+      <c r="B4" s="16">
+        <v>317</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -756,17 +805,20 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="5" width="13.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>5</v>
       </c>
       <c r="C1" s="17" t="s">
@@ -775,7 +827,7 @@
       <c r="D1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="17" t="s">
         <v>8</v>
       </c>
     </row>
@@ -783,68 +835,68 @@
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
+      <c r="B2" s="13">
+        <v>5</v>
+      </c>
+      <c r="C2" s="13">
+        <v>1</v>
+      </c>
+      <c r="D2" s="13">
+        <v>5</v>
+      </c>
+      <c r="E2" s="13">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="13">
+        <v>1</v>
+      </c>
+      <c r="C3" s="13">
+        <v>1</v>
+      </c>
+      <c r="D3" s="13">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>6</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
+      <c r="E3" s="13">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>6</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
+      <c r="B4" s="13">
+        <v>8</v>
+      </c>
+      <c r="C4" s="13">
+        <v>4</v>
+      </c>
+      <c r="D4" s="13">
+        <v>1</v>
+      </c>
+      <c r="E4" s="13">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="13">
+        <v>6</v>
+      </c>
+      <c r="C5" s="13">
         <v>2</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>8</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
+      <c r="D5" s="13">
+        <v>2</v>
+      </c>
+      <c r="E5" s="13">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -858,68 +910,133 @@
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.83203125" style="5"/>
+    <col min="1" max="1" width="30.6640625" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="10">
-        <v>0.37209999999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="10">
-        <v>0.26</v>
-      </c>
-      <c r="D3" s="13"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="10">
-        <v>0.26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="10">
-        <v>0.1052</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
-      <c r="B6" s="10"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="10"/>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="32">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="32">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="32">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="13" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="32">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" s="2" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="33">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="33">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="33">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="32">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -928,89 +1045,94 @@
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22:I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="5"/>
+    <col min="1" max="1" width="32.1640625" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="21">
+        <v>0.40397762585456803</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="21">
+        <v>0.199502796768179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="22">
+        <v>0.10689869484151647</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+      <c r="B5" s="21">
+        <v>0.12243629583592293</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="11">
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
+      <c r="B6" s="21">
+        <v>9.1982597886886258E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="11">
-        <v>0.22159999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
+      <c r="B7" s="23">
+        <v>4.7855811062771911E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="19">
-        <v>0.12670000000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="B8" s="23">
+        <v>1.5537600994406464E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="11">
-        <v>8.3000000000000004E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="11">
-        <v>7.6999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="20">
-        <v>2.4400000000000002E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="20">
-        <v>1.3299999999999999E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="20">
-        <v>1.0999999999999999E-2</v>
-      </c>
+      <c r="B9" s="23">
+        <v>9.9440646364201361E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="7.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:2" ht="7.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:2" s="2" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1025,117 +1147,118 @@
   </sheetPr>
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.5" style="5"/>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="18">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="18">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B4" s="18">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+      <c r="B5" s="19">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="9">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
+      <c r="B6" s="18">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="9">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="B7" s="19">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="9">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
+      <c r="B8" s="20">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="7">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="B9" s="20">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="9">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
+      <c r="B10" s="20">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="7">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+      <c r="B11" s="20">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="5">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
+      <c r="B12" s="20">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="5">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="5">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="5">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="5">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="5">
-        <v>158</v>
+      <c r="B13" s="20">
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -1149,186 +1272,273 @@
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="112" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.1640625" customWidth="1"/>
-    <col min="2" max="2" width="11.5" style="5"/>
+    <col min="2" max="2" width="12.5" style="4" customWidth="1"/>
+    <col min="3" max="17" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="N1" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="O1" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="P1" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q1" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="27">
+        <v>503</v>
+      </c>
+      <c r="C2" s="28">
+        <v>562</v>
+      </c>
+      <c r="D2" s="28">
+        <v>638</v>
+      </c>
+      <c r="E2" s="28">
+        <v>717</v>
+      </c>
+      <c r="F2" s="28">
+        <v>790</v>
+      </c>
+      <c r="G2" s="28">
+        <v>839</v>
+      </c>
+      <c r="H2" s="28">
+        <v>981</v>
+      </c>
+      <c r="I2" s="28">
+        <v>1123</v>
+      </c>
+      <c r="J2" s="28">
+        <v>1175</v>
+      </c>
+      <c r="K2" s="28">
+        <v>1236</v>
+      </c>
+      <c r="L2" s="28">
+        <v>1302</v>
+      </c>
+      <c r="M2" s="28">
+        <v>1341</v>
+      </c>
+      <c r="N2" s="28">
+        <f>M2+1</f>
+        <v>1342</v>
+      </c>
+      <c r="O2" s="28">
+        <f>N2+110</f>
+        <v>1452</v>
+      </c>
+      <c r="P2" s="28">
+        <f>O2+94</f>
+        <v>1546</v>
+      </c>
+      <c r="Q2" s="28">
+        <f>P2+63</f>
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="27">
+        <v>144</v>
+      </c>
+      <c r="C3" s="28">
+        <v>161</v>
+      </c>
+      <c r="D3" s="28">
+        <v>189</v>
+      </c>
+      <c r="E3" s="28">
+        <v>203</v>
+      </c>
+      <c r="F3" s="28">
+        <v>211</v>
+      </c>
+      <c r="G3" s="28">
+        <v>224</v>
+      </c>
+      <c r="H3" s="28">
+        <v>232</v>
+      </c>
+      <c r="I3" s="28">
+        <v>245</v>
+      </c>
+      <c r="J3" s="28">
+        <v>258</v>
+      </c>
+      <c r="K3" s="28">
+        <v>275</v>
+      </c>
+      <c r="L3" s="28">
+        <v>292</v>
+      </c>
+      <c r="M3" s="28">
+        <v>297</v>
+      </c>
+      <c r="N3" s="28">
+        <f>M3+1</f>
+        <v>298</v>
+      </c>
+      <c r="O3" s="28">
+        <f>N3+2</f>
+        <v>300</v>
+      </c>
+      <c r="P3" s="28">
+        <f>O3+7</f>
+        <v>307</v>
+      </c>
+      <c r="Q3" s="28">
+        <f>P3+11</f>
+        <v>318</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
+      <c r="Q4" s="28"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="21" t="s">
+      <c r="B5" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" s="21" t="s">
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="28"/>
+      <c r="P5" s="28"/>
+      <c r="Q5" s="28"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="H1" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="J1" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="K1" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="L1" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="M1" s="21" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="9">
-        <v>503</v>
-      </c>
-      <c r="C2">
-        <v>562</v>
-      </c>
-      <c r="D2">
-        <v>638</v>
-      </c>
-      <c r="E2">
-        <v>717</v>
-      </c>
-      <c r="F2">
-        <v>790</v>
-      </c>
-      <c r="G2">
-        <v>839</v>
-      </c>
-      <c r="H2">
-        <v>981</v>
-      </c>
-      <c r="I2">
-        <v>1123</v>
-      </c>
-      <c r="J2">
-        <v>1175</v>
-      </c>
-      <c r="K2">
-        <v>1236</v>
-      </c>
-      <c r="L2">
-        <v>1302</v>
-      </c>
-      <c r="M2">
-        <v>1341</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="9">
-        <v>144</v>
-      </c>
-      <c r="C3">
-        <v>161</v>
-      </c>
-      <c r="D3">
-        <v>189</v>
-      </c>
-      <c r="E3">
-        <v>203</v>
-      </c>
-      <c r="F3">
-        <v>211</v>
-      </c>
-      <c r="G3">
-        <v>224</v>
-      </c>
-      <c r="H3">
-        <v>232</v>
-      </c>
-      <c r="I3">
-        <v>245</v>
-      </c>
-      <c r="J3">
-        <v>258</v>
-      </c>
-      <c r="K3">
-        <v>275</v>
-      </c>
-      <c r="L3">
-        <v>292</v>
-      </c>
-      <c r="M3">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="11"/>
-      <c r="B7" s="7"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="11"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="11"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="11"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="28"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" s="8"/>
+      <c r="B7" s="6"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="8"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" s="8"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="8"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -1338,21 +1548,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002BE1C044AB627347BF817823C98F3378" ma:contentTypeVersion="15" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="a7fc5115c5d802368a6352c9bef00a92">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="30e0d9c9-5a01-4ada-bab5-83d0a03adf4e" xmlns:ns3="c5ab1498-896e-470f-a742-d67a3aaf8eb4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c7188ad6a712c2704da12e7f0c2e3c73" ns2:_="" ns3:_="">
     <xsd:import namespace="30e0d9c9-5a01-4ada-bab5-83d0a03adf4e"/>
@@ -1581,24 +1776,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C968D9BC-12CE-4579-9968-E3377D3993D2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9903699-3E7D-4C00-A6EB-5674F3D3403B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C655A3EA-0F88-41E4-8A14-245C9AD2A208}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1615,4 +1808,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9903699-3E7D-4C00-A6EB-5674F3D3403B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C968D9BC-12CE-4579-9968-E3377D3993D2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>